<commit_message>
Uploaded to repository for updated project plan and scope
</commit_message>
<xml_diff>
--- a/ProjectPlan/projectplan.xlsx
+++ b/ProjectPlan/projectplan.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Asit\Personal\Berkley BootCamp\Module-20 Project\nba-player-analytics\ProjectPlan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C328132-2740-49DC-80C1-D572EFF5B9F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FA84463-C1CF-46C0-8E1C-5107649F9EA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="47070" yWindow="3660" windowWidth="12300" windowHeight="11055" xr2:uid="{02B43DB1-9BF8-4CA9-885F-AB6A9EC5F607}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{02B43DB1-9BF8-4CA9-885F-AB6A9EC5F607}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan!$A$1:$H$17</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="39">
   <si>
     <t>Task Name</t>
   </si>
@@ -136,6 +139,21 @@
   </si>
   <si>
     <t>In-progress</t>
+  </si>
+  <si>
+    <t>complete</t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create scripts and upload to repository </t>
+  </si>
+  <si>
+    <t>Sample data creation (at least for 20 players in database)</t>
+  </si>
+  <si>
+    <t>Segment-2</t>
   </si>
 </sst>
 </file>
@@ -180,7 +198,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -212,19 +230,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -539,16 +567,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC7D29CE-9598-408B-82B0-D5CF3DDC2BEA}">
-  <dimension ref="A1:I23"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="29.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="29.1796875" customWidth="1"/>
+    <col min="2" max="2" width="25.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.1796875" customWidth="1"/>
     <col min="4" max="4" width="19.54296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.08984375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.7265625" bestFit="1" customWidth="1"/>
@@ -558,31 +588,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>2</v>
       </c>
     </row>
@@ -597,10 +627,18 @@
       <c r="D2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="E2" s="9">
+        <v>44403</v>
+      </c>
+      <c r="F2" s="9">
+        <v>44403</v>
+      </c>
+      <c r="G2" s="9">
+        <v>44403</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -614,10 +652,18 @@
       <c r="D3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
+      <c r="E3" s="9">
+        <v>44403</v>
+      </c>
+      <c r="F3" s="9">
+        <v>44403</v>
+      </c>
+      <c r="G3" s="9">
+        <v>44403</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -631,10 +677,18 @@
       <c r="D4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
+      <c r="E4" s="9">
+        <v>44403</v>
+      </c>
+      <c r="F4" s="9">
+        <v>44403</v>
+      </c>
+      <c r="G4" s="9">
+        <v>44403</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -648,67 +702,83 @@
       <c r="D5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
+      <c r="E5" s="8">
+        <v>44397</v>
+      </c>
+      <c r="F5" s="8">
+        <v>44403</v>
+      </c>
+      <c r="G5" s="8">
+        <v>44404</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="7" t="s">
+      <c r="B6" s="11"/>
+      <c r="C6" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="9">
-        <v>44403</v>
-      </c>
-      <c r="F6" s="9">
+      <c r="E6" s="14">
+        <v>44403</v>
+      </c>
+      <c r="F6" s="14">
         <v>44405</v>
       </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
+      <c r="G6" s="14">
+        <v>44405</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>34</v>
+      </c>
       <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="7" t="s">
+      <c r="C7" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="14">
         <v>44404</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="14">
         <v>44405</v>
       </c>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1" t="s">
+      <c r="G7" s="11"/>
+      <c r="H7" s="11" t="s">
         <v>33</v>
       </c>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="1"/>
-      <c r="B8" s="6" t="s">
+    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
+      <c r="C8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
         <v>33</v>
@@ -716,179 +786,215 @@
       <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="1"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
+      <c r="A9" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="11"/>
+      <c r="C9" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="14">
+        <v>44403</v>
+      </c>
+      <c r="F9" s="14">
+        <v>44406</v>
+      </c>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11" t="s">
+        <v>33</v>
+      </c>
       <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="7" t="s">
+      <c r="A10" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="11"/>
+      <c r="C10" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="14">
+        <v>44403</v>
+      </c>
+      <c r="F10" s="14">
         <v>44405</v>
       </c>
-      <c r="F10" s="9">
+      <c r="G10" s="14">
         <v>44405</v>
       </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
+      <c r="H10" s="11" t="s">
+        <v>34</v>
+      </c>
       <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="7" t="s">
+      <c r="A11" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="11"/>
+      <c r="C11" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
+      <c r="E11" s="14">
+        <v>44403</v>
+      </c>
+      <c r="F11" s="14">
+        <v>44405</v>
+      </c>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11" t="s">
+        <v>33</v>
+      </c>
       <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="7" t="s">
+      <c r="A12" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="11"/>
+      <c r="C12" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
+      <c r="E12" s="14">
+        <v>44403</v>
+      </c>
+      <c r="F12" s="14">
+        <v>44405</v>
+      </c>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11" t="s">
+        <v>33</v>
+      </c>
       <c r="I12" s="1"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
+      <c r="A13" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="11"/>
+      <c r="C13" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="14">
+        <v>44404</v>
+      </c>
+      <c r="F13" s="14">
+        <v>44405</v>
+      </c>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11" t="s">
+        <v>33</v>
+      </c>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
+    <row r="14" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="14">
+        <v>44404</v>
+      </c>
+      <c r="F14" s="14">
+        <v>44405</v>
+      </c>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11" t="s">
+        <v>33</v>
+      </c>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="6"/>
+    <row r="15" spans="1:9" ht="34.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="5"/>
+      <c r="B15" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="C15" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E15" s="9">
-        <v>44404</v>
-      </c>
-      <c r="F15" s="9">
-        <v>44405</v>
-      </c>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="6"/>
+    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="5"/>
       <c r="C16" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" s="9">
-        <v>44404</v>
-      </c>
-      <c r="F16" s="9">
-        <v>44405</v>
+      <c r="D16" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="8">
+        <v>44406</v>
+      </c>
+      <c r="F16" s="8">
+        <v>44409</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" s="6"/>
+    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="5"/>
       <c r="C17" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
+      <c r="D17" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="8">
+        <v>44406</v>
+      </c>
+      <c r="F17" s="8">
+        <v>44409</v>
+      </c>
       <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
+      <c r="H17" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="I17" s="1"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>23</v>
-      </c>
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -929,28 +1035,36 @@
       <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
+      <c r="A22" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="11"/>
+      <c r="C22" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="14">
+        <v>44405</v>
+      </c>
+      <c r="F22" s="14">
+        <v>44405</v>
+      </c>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11" t="s">
+        <v>33</v>
+      </c>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-    </row>
   </sheetData>
+  <autoFilter ref="A1:H17" xr:uid="{DC1799C0-9CC6-4F84-A86B-D6484F16B5FF}">
+    <filterColumn colId="5">
+      <filters>
+        <dateGroupItem year="2021" month="7" dateTimeGrouping="month"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated the project plan on 08/02
</commit_message>
<xml_diff>
--- a/ProjectPlan/projectplan.xlsx
+++ b/ProjectPlan/projectplan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Asit\Personal\Berkley BootCamp\Module-20 Project\nba-player-analytics\ProjectPlan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0FE3818B-CDD5-474F-AB5D-852550AAA7FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E87E1A-83A3-423C-B859-CEE1496DC4FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{02B43DB1-9BF8-4CA9-885F-AB6A9EC5F607}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Plan" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan!$A$1:$H$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan!$A$1:$H$24</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="54">
   <si>
     <t>Task Name</t>
   </si>
@@ -60,9 +60,6 @@
     <t>Check granularity and quality</t>
   </si>
   <si>
-    <t>Finalize ETL steps</t>
-  </si>
-  <si>
     <t>Finalize scope</t>
   </si>
   <si>
@@ -154,6 +151,54 @@
   </si>
   <si>
     <t>Segment-2</t>
+  </si>
+  <si>
+    <t>Sample data in Player Statistics</t>
+  </si>
+  <si>
+    <t>Sample data in Player Salary</t>
+  </si>
+  <si>
+    <t>Sample data required for Dashboard</t>
+  </si>
+  <si>
+    <t>ETL</t>
+  </si>
+  <si>
+    <t>ETL - for Player Statistics - Build</t>
+  </si>
+  <si>
+    <t>ETL - for Player Statistics - Review &amp; Merge</t>
+  </si>
+  <si>
+    <t>ETL - for Player Salary - Build</t>
+  </si>
+  <si>
+    <t>ETL - for Player Salary - Review &amp; Merge</t>
+  </si>
+  <si>
+    <t>Sample data creation</t>
+  </si>
+  <si>
+    <t>Dashboard blue printing</t>
+  </si>
+  <si>
+    <t>Dashboard Mockup - build</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M/C Learning </t>
+  </si>
+  <si>
+    <t>Clustering - enhancement</t>
+  </si>
+  <si>
+    <t>Supervised Learning - Build</t>
+  </si>
+  <si>
+    <t>Clustering - enhancement - Review &amp; Merge</t>
+  </si>
+  <si>
+    <t>Supervised Learning - Review &amp; Merge</t>
   </si>
 </sst>
 </file>
@@ -198,12 +243,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -215,6 +260,19 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -246,13 +304,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -567,17 +623,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC7D29CE-9598-408B-82B0-D5CF3DDC2BEA}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="29.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.1796875" customWidth="1"/>
     <col min="4" max="4" width="19.54296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.08984375" bestFit="1" customWidth="1"/>
@@ -592,22 +649,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>4</v>
       </c>
       <c r="E1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="7" t="s">
-        <v>26</v>
-      </c>
       <c r="G1" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>1</v>
@@ -618,14 +675,14 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E2" s="9">
         <v>44403</v>
@@ -637,20 +694,20 @@
         <v>44403</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3" s="9">
         <v>44403</v>
@@ -662,20 +719,20 @@
         <v>44403</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E4" s="9">
         <v>44403</v>
@@ -687,7 +744,7 @@
         <v>44403</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I4" s="2"/>
     </row>
@@ -697,10 +754,10 @@
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5" s="8">
         <v>44397</v>
@@ -712,231 +769,231 @@
         <v>44404</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="13" t="s">
+      <c r="B6" s="5"/>
+      <c r="C6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="11">
+        <v>44403</v>
+      </c>
+      <c r="F6" s="11">
+        <v>44405</v>
+      </c>
+      <c r="G6" s="11">
+        <v>44405</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="14">
-        <v>44403</v>
-      </c>
-      <c r="F6" s="14">
+      <c r="E7" s="11">
+        <v>44404</v>
+      </c>
+      <c r="F7" s="11">
         <v>44405</v>
       </c>
-      <c r="G6" s="14">
-        <v>44405</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="14">
-        <v>44404</v>
-      </c>
-      <c r="F7" s="14">
-        <v>44405</v>
-      </c>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11" t="s">
+      <c r="G7" s="5"/>
+      <c r="H7" s="5" t="s">
         <v>33</v>
       </c>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="5"/>
       <c r="B8" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="11">
+        <v>44403</v>
+      </c>
+      <c r="F9" s="11">
+        <v>44406</v>
+      </c>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="11" t="s">
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="14">
-        <v>44403</v>
-      </c>
-      <c r="F9" s="14">
-        <v>44406</v>
-      </c>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11" t="s">
+      <c r="B10" s="5"/>
+      <c r="C10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="11">
+        <v>44403</v>
+      </c>
+      <c r="F10" s="11">
+        <v>44405</v>
+      </c>
+      <c r="G10" s="11">
+        <v>44405</v>
+      </c>
+      <c r="H10" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="11" t="s">
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="11">
+        <v>44403</v>
+      </c>
+      <c r="F11" s="11">
+        <v>44405</v>
+      </c>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="11">
+        <v>44403</v>
+      </c>
+      <c r="F12" s="11">
+        <v>44405</v>
+      </c>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="14">
-        <v>44403</v>
-      </c>
-      <c r="F10" s="14">
+      <c r="B13" s="5"/>
+      <c r="C13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="11">
+        <v>44404</v>
+      </c>
+      <c r="F13" s="11">
         <v>44405</v>
       </c>
-      <c r="G10" s="14">
+      <c r="G13" s="5"/>
+      <c r="H13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="11">
+        <v>44404</v>
+      </c>
+      <c r="F14" s="11">
         <v>44405</v>
       </c>
-      <c r="H10" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="11"/>
-      <c r="C11" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="14">
-        <v>44403</v>
-      </c>
-      <c r="F11" s="14">
-        <v>44405</v>
-      </c>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11" t="s">
+      <c r="G14" s="5"/>
+      <c r="H14" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" s="14">
-        <v>44403</v>
-      </c>
-      <c r="F12" s="14">
-        <v>44405</v>
-      </c>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="14">
-        <v>44404</v>
-      </c>
-      <c r="F13" s="14">
-        <v>44405</v>
-      </c>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="14">
-        <v>44404</v>
-      </c>
-      <c r="F14" s="14">
-        <v>44405</v>
-      </c>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11" t="s">
-        <v>33</v>
-      </c>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" ht="34.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5"/>
       <c r="B15" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
@@ -944,16 +1001,16 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E16" s="8">
         <v>44406</v>
@@ -963,20 +1020,20 @@
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E17" s="8">
         <v>44406</v>
@@ -986,85 +1043,282 @@
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I17" s="1"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
+      <c r="A18" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="13">
+        <v>44410</v>
+      </c>
+      <c r="F18" s="13">
+        <v>44413</v>
+      </c>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="15"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
+      <c r="A19" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="13">
+        <v>44414</v>
+      </c>
+      <c r="F19" s="13">
+        <v>44414</v>
+      </c>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="15"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
+      <c r="A20" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="13">
+        <v>44410</v>
+      </c>
+      <c r="F20" s="13">
+        <v>44413</v>
+      </c>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="15"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
+      <c r="A21" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="13">
+        <v>44414</v>
+      </c>
+      <c r="F21" s="13">
+        <v>44414</v>
+      </c>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="15"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A22" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22" s="11"/>
+      <c r="A22" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>38</v>
+      </c>
       <c r="C22" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D22" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="13">
+        <v>44411</v>
+      </c>
+      <c r="F22" s="13">
+        <v>44411</v>
+      </c>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="15"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A23" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="13">
+        <v>44411</v>
+      </c>
+      <c r="F23" s="13">
+        <v>44411</v>
+      </c>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="15"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A24" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E24" s="13">
+        <v>44411</v>
+      </c>
+      <c r="F24" s="13">
+        <v>44411</v>
+      </c>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A25" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25" s="13">
+        <v>44410</v>
+      </c>
+      <c r="F25" s="13">
+        <v>44413</v>
+      </c>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A26" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="13">
+        <v>44410</v>
+      </c>
+      <c r="F26" s="13">
+        <v>44412</v>
+      </c>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A27" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="E22" s="14">
-        <v>44405</v>
-      </c>
-      <c r="F22" s="14">
-        <v>44405</v>
-      </c>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="I22" s="1"/>
+      <c r="E27" s="13">
+        <v>44413</v>
+      </c>
+      <c r="F27" s="13">
+        <v>44413</v>
+      </c>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A28" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" s="13">
+        <v>44413</v>
+      </c>
+      <c r="F28" s="13">
+        <v>44415</v>
+      </c>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A29" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" s="13">
+        <v>44416</v>
+      </c>
+      <c r="F29" s="13">
+        <v>44416</v>
+      </c>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H17" xr:uid="{DC1799C0-9CC6-4F84-A86B-D6484F16B5FF}">
-    <filterColumn colId="5">
-      <filters>
-        <dateGroupItem year="2021" month="7" dateTimeGrouping="month"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:H24" xr:uid="{DC1799C0-9CC6-4F84-A86B-D6484F16B5FF}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>

</xml_diff>